<commit_message>
sprint 108 manual testcases
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Inventory Final listing testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Inventory Final listing testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48B8BBE-A12E-44CB-B306-7BAF785D98A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DF7D90-B711-4650-ADD6-31D22A91D109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t>SL. No</t>
   </si>
@@ -138,45 +138,6 @@
   </si>
   <si>
     <t>View Inventory menu page</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Click on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>"Settings "</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">As per expected, When </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>"Settings"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> is clicked, a modal appeared. User should tick the display custom SKU name instead of original name ,if they want to see the custom names rather than the original name</t>
-    </r>
   </si>
   <si>
     <r>
@@ -548,41 +509,6 @@
   </si>
   <si>
     <t>it displayed the particular outlet details</t>
-  </si>
-  <si>
-    <r>
-      <t>1.When</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> "Settings"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> is clicked, a modal appears. User should tick the display custom SKU name instead of original name ,if they want to see the custom names rather than the original name 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2. Click Save button it gets saved</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -713,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -738,16 +664,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1061,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,58 +1104,58 @@
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="11" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="11" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="11" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
-        <v>6</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="21" t="s">
+      <c r="F7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1252,13 +1170,13 @@
         <v>23</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>13</v>
@@ -1268,20 +1186,20 @@
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>13</v>
@@ -1291,20 +1209,20 @@
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>46</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>13</v>
@@ -1314,20 +1232,20 @@
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>13</v>
@@ -1337,20 +1255,20 @@
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>50</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>13</v>
@@ -1360,125 +1278,103 @@
       <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="G13" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="E14" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
-        <v>13</v>
-      </c>
-      <c r="B14" s="19" t="s">
+      <c r="F14" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26">
-        <v>14</v>
-      </c>
-      <c r="B15" s="19" t="s">
+      <c r="D15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D16" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26">
-        <v>15</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26">
-        <v>16</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="95.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
+      <c r="G16" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="95.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:7" ht="95.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Manual testcases of sprint114
</commit_message>
<xml_diff>
--- a/Buyer hub/Inventory/Manual testcases/Inventory Final listing testcases.xlsx
+++ b/Buyer hub/Inventory/Manual testcases/Inventory Final listing testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zm-buyerautomation\Buyer hub\Inventory\Manual testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DF7D90-B711-4650-ADD6-31D22A91D109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7974C94-7E01-4989-BC80-B82F10B4BDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
   <si>
     <t>SL. No</t>
   </si>
@@ -509,6 +509,25 @@
   </si>
   <si>
     <t>it displayed the particular outlet details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click the Checkbox </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Once click the Checkbox , a button will appear at the top to allow users to  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Clear and Download inventory report"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -977,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:G17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,7 +1247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1238,20 +1257,16 @@
       <c r="C11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>47</v>
+      <c r="D11" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="11" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1265,16 +1280,16 @@
         <v>47</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="11" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1285,20 +1300,20 @@
         <v>25</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+        <v>47</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
@@ -1308,20 +1323,20 @@
         <v>25</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+    <row r="15" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -1330,20 +1345,20 @@
       <c r="C15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>33</v>
+      <c r="D15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>56</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>15</v>
       </c>
@@ -1353,11 +1368,11 @@
       <c r="C16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="21" t="s">
-        <v>35</v>
+      <c r="D16" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>34</v>
@@ -1366,15 +1381,38 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="95.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:7" ht="95.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
+    <row r="17" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="95.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:7" ht="95.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="15"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>